<commit_message>
Update control decision matrix
</commit_message>
<xml_diff>
--- a/Documentation/Report/Control decision matrix.xlsx
+++ b/Documentation/Report/Control decision matrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\advik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/159ea1024a16f528/Documents/Imperial/YEAR_2/Design_Project/EEEBalanceBug/Documentation/Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58C6651B-3EF9-4AEC-876C-1BA66833159C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{862C2E0D-0FD1-448A-A865-5D3D343C3156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{AEAF3C4F-CC49-454A-BDAC-A062DB354F25}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Weight</t>
   </si>
@@ -94,13 +94,25 @@
   </si>
   <si>
     <t>Performance</t>
+  </si>
+  <si>
+    <t>Computational Efficiency</t>
+  </si>
+  <si>
+    <t>Implementation Efficiency</t>
+  </si>
+  <si>
+    <t>([1-5] lower is better)</t>
+  </si>
+  <si>
+    <t>old:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,16 +120,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -223,11 +273,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -256,20 +333,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F8E860-DC74-4B3E-BAD1-A019D00882CF}">
-  <dimension ref="B2:K7"/>
+  <dimension ref="B2:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -600,24 +707,24 @@
     <col min="11" max="11" width="16.1328125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B2" s="14" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="17"/>
-    </row>
-    <row r="3" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="13" t="s">
         <v>4</v>
       </c>
@@ -634,53 +741,53 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" s="4">
         <v>3</v>
       </c>
       <c r="D4" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="5">
-        <v>2</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>5</v>
       </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B5" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5">
         <v>2</v>
       </c>
       <c r="D5" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F5" s="8">
         <v>3</v>
       </c>
       <c r="G5" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H5" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
@@ -688,7 +795,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -697,47 +804,180 @@
         <v>3</v>
       </c>
       <c r="G6" s="2">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2">
         <v>1</v>
       </c>
-      <c r="H6" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B7" s="16" t="s">
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="9" cm="1">
         <f t="array" ref="D7">SUM(C4:C6*D4:D6)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E7" s="7" cm="1">
         <f t="array" ref="E7">SUM(C4:C6*E4:E6)</f>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F7" s="9" cm="1">
         <f t="array" ref="F7">SUM(C4:C6*F4:F6)</f>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G7" s="6" cm="1">
         <f t="array" ref="G7">SUM(G4:G6*C4:C6)</f>
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="H7" s="6" cm="1">
         <f t="array" ref="H7">SUM(H4:H6*C4:C6)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="26.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="20"/>
+      <c r="I12" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B13" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="22">
+        <v>3</v>
+      </c>
+      <c r="D13" s="27">
+        <v>2</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="22">
+        <v>1</v>
+      </c>
+      <c r="G13" s="22">
+        <v>2</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="22">
+        <v>5</v>
+      </c>
+      <c r="J13" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B14" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="24">
+        <v>2</v>
+      </c>
+      <c r="D14" s="28">
+        <v>4</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="24">
+        <v>4</v>
+      </c>
+      <c r="G14" s="24">
+        <v>3</v>
+      </c>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24">
+        <v>5</v>
+      </c>
+      <c r="J14" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B15" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="22">
+        <v>1</v>
+      </c>
+      <c r="D15" s="26">
+        <v>2</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="22">
+        <v>3</v>
+      </c>
+      <c r="G15" s="22">
+        <v>3</v>
+      </c>
+      <c r="H15" s="23"/>
+      <c r="I15" s="22">
+        <v>1</v>
+      </c>
+      <c r="J15" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B16" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="28">
+        <v>16</v>
+      </c>
+      <c r="E16" s="28"/>
+      <c r="F16" s="24">
+        <v>14</v>
+      </c>
+      <c r="G16" s="24">
+        <v>15</v>
+      </c>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24">
+        <v>26</v>
+      </c>
+      <c r="J16" s="24">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="9">
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="D2:H2"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="C12:D12"/>
   </mergeCells>
-  <conditionalFormatting sqref="H4:H6">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="D4:G6">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -746,8 +986,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:G6">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="H4:H6">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>